<commit_message>
Playing with parameter give only 7 wrong image
</commit_message>
<xml_diff>
--- a/Contour/Resources/fail(correct).xlsx
+++ b/Contour/Resources/fail(correct).xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
   <si>
     <t>C:\EDU\Orient\bin\Debug\..\..\base\acts\Р°РєС‚ 2.jpg</t>
   </si>
@@ -209,6 +209,12 @@
   </si>
   <si>
     <t>C:\EDU\Orient\bin\Debug\..\..\base\more\04b03f6918e33aa3977eabc66fe26529_1_NA.JPG</t>
+  </si>
+  <si>
+    <t>плохой</t>
+  </si>
+  <si>
+    <t>бинаризация</t>
   </si>
 </sst>
 </file>
@@ -1049,38 +1055,41 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="1"/>
-  <dimension ref="A2:J66"/>
+  <dimension ref="A2:P65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I66" sqref="I66"/>
+      <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="16" max="16" width="13.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="1:10" hidden="1">
+    <row r="2" spans="1:16" hidden="1">
       <c r="A2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2">
+        <v>16</v>
+      </c>
+      <c r="D2">
+        <v>5</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
         <v>18</v>
       </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>3</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2">
-        <v>23</v>
-      </c>
       <c r="H2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -1089,7 +1098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" hidden="1">
+    <row r="3" spans="1:16" hidden="1">
       <c r="A3">
         <v>12</v>
       </c>
@@ -1106,13 +1115,13 @@
         <v>11</v>
       </c>
       <c r="F3">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G3">
         <v>23</v>
       </c>
       <c r="H3">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -1121,18 +1130,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" hidden="1">
+    <row r="4" spans="1:16" hidden="1">
       <c r="A4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C4">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D4">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="E4">
         <v>3</v>
@@ -1141,42 +1150,42 @@
         <v>1</v>
       </c>
       <c r="G4">
+        <v>25</v>
+      </c>
+      <c r="H4">
+        <v>18</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" hidden="1">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>21</v>
+      </c>
+      <c r="D5">
+        <v>16</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
         <v>23</v>
       </c>
-      <c r="H4">
-        <v>13</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-      <c r="J4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" hidden="1">
-      <c r="A5">
-        <v>1</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <v>23</v>
-      </c>
-      <c r="D5">
-        <v>11</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <v>25</v>
-      </c>
       <c r="H5">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="I5">
         <v>0</v>
@@ -1185,15 +1194,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:10" hidden="1">
+    <row r="6" spans="1:16" hidden="1">
       <c r="A6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C6">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="D6">
         <v>5</v>
@@ -1202,13 +1211,13 @@
         <v>0</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G6">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="H6">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="I6">
         <v>0</v>
@@ -1217,7 +1226,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:10" hidden="1">
+    <row r="7" spans="1:16" hidden="1">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1234,13 +1243,13 @@
         <v>6</v>
       </c>
       <c r="F7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G7">
         <v>13</v>
       </c>
       <c r="H7">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I7">
         <v>0</v>
@@ -1249,30 +1258,30 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:10" hidden="1">
+    <row r="8" spans="1:16" hidden="1">
       <c r="A8">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="B8">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="C8">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D8">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E8">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="F8">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="G8">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="H8">
-        <v>87</v>
+        <v>56</v>
       </c>
       <c r="I8">
         <v>0</v>
@@ -1281,30 +1290,30 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:10" hidden="1">
+    <row r="9" spans="1:16" hidden="1">
       <c r="A9">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C9">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="D9">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E9">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F9">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="G9">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="H9">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="I9">
         <v>0</v>
@@ -1313,9 +1322,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:16">
       <c r="A10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B10">
         <v>2</v>
@@ -1327,7 +1336,7 @@
         <v>0</v>
       </c>
       <c r="E10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F10">
         <v>1</v>
@@ -1344,31 +1353,34 @@
       <c r="J10" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" hidden="1">
+      <c r="P10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" hidden="1">
       <c r="A11">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B11">
         <v>2</v>
       </c>
       <c r="C11">
+        <v>21</v>
+      </c>
+      <c r="D11">
+        <v>10</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
         <v>25</v>
       </c>
-      <c r="D11">
-        <v>20</v>
-      </c>
-      <c r="E11">
-        <v>1</v>
-      </c>
-      <c r="F11">
-        <v>1</v>
-      </c>
-      <c r="G11">
-        <v>28</v>
-      </c>
       <c r="H11">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="I11">
         <v>0</v>
@@ -1377,7 +1389,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:10" hidden="1">
+    <row r="12" spans="1:16" hidden="1">
       <c r="A12">
         <v>0</v>
       </c>
@@ -1385,22 +1397,22 @@
         <v>2</v>
       </c>
       <c r="C12">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D12">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="E12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F12">
         <v>3</v>
       </c>
       <c r="G12">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="H12">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="I12">
         <v>0</v>
@@ -1409,27 +1421,27 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:10" hidden="1">
+    <row r="13" spans="1:16" hidden="1">
       <c r="A13">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B13">
         <v>2</v>
       </c>
       <c r="C13">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D13">
         <v>5</v>
       </c>
       <c r="E13">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F13">
         <v>2</v>
       </c>
       <c r="G13">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="H13">
         <v>9</v>
@@ -1441,18 +1453,18 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:10" hidden="1">
+    <row r="14" spans="1:16" hidden="1">
       <c r="A14">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B14">
         <v>1</v>
       </c>
       <c r="C14">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D14">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E14">
         <v>2</v>
@@ -1461,10 +1473,10 @@
         <v>1</v>
       </c>
       <c r="G14">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="H14">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I14">
         <v>0</v>
@@ -1473,30 +1485,30 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:10" hidden="1">
+    <row r="15" spans="1:16" hidden="1">
       <c r="A15">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15">
+        <v>43</v>
+      </c>
+      <c r="D15">
         <v>7</v>
       </c>
-      <c r="C15">
-        <v>44</v>
-      </c>
-      <c r="D15">
-        <v>10</v>
-      </c>
       <c r="E15">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F15">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G15">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="H15">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="I15">
         <v>0</v>
@@ -1505,30 +1517,30 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:10" hidden="1">
+    <row r="16" spans="1:16" hidden="1">
       <c r="A16">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="B16">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C16">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D16">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E16">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="F16">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="G16">
-        <v>90</v>
+        <v>61</v>
       </c>
       <c r="H16">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="I16">
         <v>0</v>
@@ -1537,27 +1549,27 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:10" hidden="1">
+    <row r="17" spans="1:16" hidden="1">
       <c r="A17">
+        <v>9</v>
+      </c>
+      <c r="B17">
+        <v>7</v>
+      </c>
+      <c r="C17">
+        <v>17</v>
+      </c>
+      <c r="D17">
         <v>13</v>
       </c>
-      <c r="B17">
-        <v>6</v>
-      </c>
-      <c r="C17">
-        <v>25</v>
-      </c>
-      <c r="D17">
-        <v>15</v>
-      </c>
       <c r="E17">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="F17">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G17">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="H17">
         <v>28</v>
@@ -1569,30 +1581,30 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:10" hidden="1">
+    <row r="18" spans="1:16" hidden="1">
       <c r="A18">
+        <v>10</v>
+      </c>
+      <c r="B18">
+        <v>5</v>
+      </c>
+      <c r="C18">
+        <v>25</v>
+      </c>
+      <c r="D18">
+        <v>9</v>
+      </c>
+      <c r="E18">
         <v>11</v>
       </c>
-      <c r="B18">
-        <v>9</v>
-      </c>
-      <c r="C18">
-        <v>23</v>
-      </c>
-      <c r="D18">
-        <v>10</v>
-      </c>
-      <c r="E18">
-        <v>7</v>
-      </c>
       <c r="F18">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G18">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="H18">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="I18">
         <v>0</v>
@@ -1601,30 +1613,30 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:10" hidden="1">
+    <row r="19" spans="1:16" hidden="1">
       <c r="A19">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B19">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C19">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D19">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E19">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F19">
         <v>3</v>
       </c>
       <c r="G19">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="H19">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I19">
         <v>0</v>
@@ -1633,30 +1645,30 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:10" hidden="1">
+    <row r="20" spans="1:16" hidden="1">
       <c r="A20">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B20">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C20">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D20">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E20">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F20">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G20">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H20">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="I20">
         <v>0</v>
@@ -1665,30 +1677,30 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:10" hidden="1">
+    <row r="21" spans="1:16" hidden="1">
       <c r="A21">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B21">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C21">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="D21">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="E21">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="F21">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="G21">
-        <v>79</v>
+        <v>57</v>
       </c>
       <c r="H21">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="I21">
         <v>0</v>
@@ -1697,30 +1709,30 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:10" hidden="1">
+    <row r="22" spans="1:16" hidden="1">
       <c r="A22">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B22">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C22">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="D22">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="E22">
         <v>6</v>
       </c>
       <c r="F22">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="G22">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="H22">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="I22">
         <v>0</v>
@@ -1729,30 +1741,30 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:10" hidden="1">
+    <row r="23" spans="1:16" hidden="1">
       <c r="A23">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="B23">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C23">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="D23">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E23">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F23">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G23">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H23">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I23">
         <v>0</v>
@@ -1761,30 +1773,30 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:10" hidden="1">
+    <row r="24" spans="1:16" hidden="1">
       <c r="A24">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B24">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C24">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D24">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="E24">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F24">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G24">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="H24">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="I24">
         <v>0</v>
@@ -1793,30 +1805,30 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:10" hidden="1">
+    <row r="25" spans="1:16" hidden="1">
       <c r="A25">
+        <v>1</v>
+      </c>
+      <c r="B25">
         <v>4</v>
       </c>
-      <c r="B25">
-        <v>2</v>
-      </c>
       <c r="C25">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D25">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E25">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F25">
         <v>3</v>
       </c>
       <c r="G25">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="H25">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I25">
         <v>0</v>
@@ -1825,30 +1837,30 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:10" hidden="1">
+    <row r="26" spans="1:16" hidden="1">
       <c r="A26">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="B26">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C26">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="D26">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="E26">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F26">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G26">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="H26">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="I26">
         <v>0</v>
@@ -1857,30 +1869,30 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:10" hidden="1">
+    <row r="27" spans="1:16" hidden="1">
       <c r="A27">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B27">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C27">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="D27">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E27">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F27">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G27">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="H27">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="I27">
         <v>0</v>
@@ -1889,27 +1901,27 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:10" hidden="1">
+    <row r="28" spans="1:16" hidden="1">
       <c r="A28">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="B28">
         <v>3</v>
       </c>
       <c r="C28">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D28">
         <v>16</v>
       </c>
       <c r="E28">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F28">
         <v>3</v>
       </c>
       <c r="G28">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="H28">
         <v>22</v>
@@ -1921,30 +1933,30 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:10" hidden="1">
+    <row r="29" spans="1:16" hidden="1">
       <c r="A29">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="B29">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C29">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="D29">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="E29">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="F29">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="G29">
-        <v>86</v>
+        <v>59</v>
       </c>
       <c r="H29">
-        <v>78</v>
+        <v>53</v>
       </c>
       <c r="I29">
         <v>0</v>
@@ -1953,30 +1965,30 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:16">
       <c r="A30">
+        <v>3</v>
+      </c>
+      <c r="B30">
         <v>4</v>
       </c>
-      <c r="B30">
-        <v>3</v>
-      </c>
       <c r="C30">
+        <v>26</v>
+      </c>
+      <c r="D30">
+        <v>43</v>
+      </c>
+      <c r="E30">
+        <v>2</v>
+      </c>
+      <c r="F30">
+        <v>2</v>
+      </c>
+      <c r="G30">
         <v>31</v>
       </c>
-      <c r="D30">
-        <v>41</v>
-      </c>
-      <c r="E30">
-        <v>1</v>
-      </c>
-      <c r="F30">
-        <v>3</v>
-      </c>
-      <c r="G30">
-        <v>36</v>
-      </c>
       <c r="H30">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="I30">
         <v>1</v>
@@ -1984,10 +1996,13 @@
       <c r="J30" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" hidden="1">
+      <c r="P30" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" hidden="1">
       <c r="A31">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B31">
         <v>0</v>
@@ -1996,7 +2011,7 @@
         <v>18</v>
       </c>
       <c r="D31">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E31">
         <v>1</v>
@@ -2005,10 +2020,10 @@
         <v>0</v>
       </c>
       <c r="G31">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H31">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="I31">
         <v>0</v>
@@ -2017,33 +2032,33 @@
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:10" hidden="1">
+    <row r="32" spans="1:16">
       <c r="A32">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="B32">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C32">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="D32">
         <v>13</v>
       </c>
       <c r="E32">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="F32">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G32">
-        <v>72</v>
+        <v>34</v>
       </c>
       <c r="H32">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="I32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J32" t="s">
         <v>30</v>
@@ -2051,28 +2066,28 @@
     </row>
     <row r="33" spans="1:10" hidden="1">
       <c r="A33">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B33">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C33">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D33">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E33">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F33">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="G33">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="H33">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="I33">
         <v>0</v>
@@ -2083,28 +2098,28 @@
     </row>
     <row r="34" spans="1:10" hidden="1">
       <c r="A34">
+        <v>13</v>
+      </c>
+      <c r="B34">
         <v>19</v>
       </c>
-      <c r="B34">
-        <v>20</v>
-      </c>
       <c r="C34">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="D34">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="E34">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F34">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="G34">
-        <v>86</v>
+        <v>64</v>
       </c>
       <c r="H34">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="I34">
         <v>0</v>
@@ -2115,28 +2130,28 @@
     </row>
     <row r="35" spans="1:10" hidden="1">
       <c r="A35">
+        <v>1</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="C35">
+        <v>3</v>
+      </c>
+      <c r="D35">
+        <v>3</v>
+      </c>
+      <c r="E35">
+        <v>2</v>
+      </c>
+      <c r="F35">
+        <v>0</v>
+      </c>
+      <c r="G35">
+        <v>6</v>
+      </c>
+      <c r="H35">
         <v>4</v>
-      </c>
-      <c r="B35">
-        <v>2</v>
-      </c>
-      <c r="C35">
-        <v>4</v>
-      </c>
-      <c r="D35">
-        <v>4</v>
-      </c>
-      <c r="E35">
-        <v>3</v>
-      </c>
-      <c r="F35">
-        <v>0</v>
-      </c>
-      <c r="G35">
-        <v>11</v>
-      </c>
-      <c r="H35">
-        <v>6</v>
       </c>
       <c r="I35">
         <v>0</v>
@@ -2145,65 +2160,65 @@
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:10">
+    <row r="36" spans="1:10" hidden="1">
       <c r="A36">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C36">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D36">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="E36">
         <v>2</v>
       </c>
       <c r="F36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G36">
+        <v>25</v>
+      </c>
+      <c r="H36">
         <v>20</v>
       </c>
-      <c r="H36">
-        <v>23</v>
-      </c>
       <c r="I36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J36" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="1:10">
+    <row r="37" spans="1:10" hidden="1">
       <c r="A37">
         <v>4</v>
       </c>
       <c r="B37">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C37">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="D37">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="E37">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F37">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G37">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="H37">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="I37">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J37" t="s">
         <v>35</v>
@@ -2211,28 +2226,28 @@
     </row>
     <row r="38" spans="1:10" hidden="1">
       <c r="A38">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="B38">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C38">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D38">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="E38">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="F38">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="G38">
-        <v>88</v>
+        <v>65</v>
       </c>
       <c r="H38">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="I38">
         <v>0</v>
@@ -2243,28 +2258,28 @@
     </row>
     <row r="39" spans="1:10" hidden="1">
       <c r="A39">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B39">
         <v>0</v>
       </c>
       <c r="C39">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D39">
+        <v>4</v>
+      </c>
+      <c r="E39">
+        <v>0</v>
+      </c>
+      <c r="F39">
+        <v>0</v>
+      </c>
+      <c r="G39">
         <v>6</v>
       </c>
-      <c r="E39">
-        <v>0</v>
-      </c>
-      <c r="F39">
-        <v>1</v>
-      </c>
-      <c r="G39">
-        <v>11</v>
-      </c>
       <c r="H39">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="I39">
         <v>0</v>
@@ -2275,28 +2290,28 @@
     </row>
     <row r="40" spans="1:10">
       <c r="A40">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B40">
         <v>0</v>
       </c>
       <c r="C40">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D40">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="E40">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F40">
         <v>1</v>
       </c>
       <c r="G40">
+        <v>23</v>
+      </c>
+      <c r="H40">
         <v>28</v>
-      </c>
-      <c r="H40">
-        <v>34</v>
       </c>
       <c r="I40">
         <v>1</v>
@@ -2313,22 +2328,22 @@
         <v>0</v>
       </c>
       <c r="C41">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D41">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E41">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F41">
         <v>0</v>
       </c>
       <c r="G41">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H41">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="I41">
         <v>1</v>
@@ -2337,97 +2352,97 @@
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="1:10">
+    <row r="42" spans="1:10" hidden="1">
       <c r="A42">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B42">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C42">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D42">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E42">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F42">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G42">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="H42">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="I42">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J42" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:10">
+    <row r="43" spans="1:10" hidden="1">
       <c r="A43">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B43">
+        <v>1</v>
+      </c>
+      <c r="C43">
+        <v>5</v>
+      </c>
+      <c r="D43">
         <v>3</v>
       </c>
-      <c r="C43">
-        <v>2</v>
-      </c>
-      <c r="D43">
-        <v>2</v>
-      </c>
       <c r="E43">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F43">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G43">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H43">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="I43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J43" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="44" spans="1:10" hidden="1">
+    <row r="44" spans="1:10">
       <c r="A44">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B44">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C44">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="D44">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E44">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F44">
         <v>7</v>
       </c>
       <c r="G44">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="H44">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="I44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J44" t="s">
         <v>42</v>
@@ -2438,25 +2453,25 @@
         <v>9</v>
       </c>
       <c r="B45">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C45">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="D45">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E45">
         <v>9</v>
       </c>
       <c r="F45">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G45">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="H45">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="I45">
         <v>0</v>
@@ -2467,28 +2482,28 @@
     </row>
     <row r="46" spans="1:10" hidden="1">
       <c r="A46">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B46">
         <v>2</v>
       </c>
       <c r="C46">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D46">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E46">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F46">
         <v>2</v>
       </c>
       <c r="G46">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="H46">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I46">
         <v>0</v>
@@ -2499,28 +2514,28 @@
     </row>
     <row r="47" spans="1:10" hidden="1">
       <c r="A47">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B47">
         <v>0</v>
       </c>
       <c r="C47">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D47">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E47">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F47">
         <v>0</v>
       </c>
       <c r="G47">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="H47">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="I47">
         <v>0</v>
@@ -2531,13 +2546,13 @@
     </row>
     <row r="48" spans="1:10" hidden="1">
       <c r="A48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B48">
         <v>0</v>
       </c>
       <c r="C48">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D48">
         <v>7</v>
@@ -2549,7 +2564,7 @@
         <v>0</v>
       </c>
       <c r="G48">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="H48">
         <v>7</v>
@@ -2563,28 +2578,28 @@
     </row>
     <row r="49" spans="1:10" hidden="1">
       <c r="A49">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B49">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C49">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="D49">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E49">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F49">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G49">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="H49">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="I49">
         <v>0</v>
@@ -2598,25 +2613,25 @@
         <v>2</v>
       </c>
       <c r="B50">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C50">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="D50">
-        <v>55</v>
+        <v>33</v>
       </c>
       <c r="E50">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="F50">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="G50">
-        <v>84</v>
+        <v>63</v>
       </c>
       <c r="H50">
-        <v>76</v>
+        <v>43</v>
       </c>
       <c r="I50">
         <v>0</v>
@@ -2633,22 +2648,22 @@
         <v>0</v>
       </c>
       <c r="C51">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D51">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E51">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F51">
         <v>0</v>
       </c>
       <c r="G51">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H51">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I51">
         <v>0</v>
@@ -2659,28 +2674,28 @@
     </row>
     <row r="52" spans="1:10" hidden="1">
       <c r="A52">
+        <v>4</v>
+      </c>
+      <c r="B52">
+        <v>3</v>
+      </c>
+      <c r="C52">
+        <v>17</v>
+      </c>
+      <c r="D52">
         <v>11</v>
       </c>
-      <c r="B52">
-        <v>4</v>
-      </c>
-      <c r="C52">
-        <v>21</v>
-      </c>
-      <c r="D52">
-        <v>6</v>
-      </c>
       <c r="E52">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="F52">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G52">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="H52">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="I52">
         <v>0</v>
@@ -2691,16 +2706,16 @@
     </row>
     <row r="53" spans="1:10" hidden="1">
       <c r="A53">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B53">
         <v>1</v>
       </c>
       <c r="C53">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D53">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E53">
         <v>1</v>
@@ -2709,10 +2724,10 @@
         <v>0</v>
       </c>
       <c r="G53">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="H53">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I53">
         <v>0</v>
@@ -2729,10 +2744,10 @@
         <v>0</v>
       </c>
       <c r="C54">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="D54">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="E54">
         <v>0</v>
@@ -2741,10 +2756,10 @@
         <v>0</v>
       </c>
       <c r="G54">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="H54">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="I54">
         <v>0</v>
@@ -2753,7 +2768,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="55" spans="1:10">
+    <row r="55" spans="1:10" hidden="1">
       <c r="A55">
         <v>0</v>
       </c>
@@ -2761,25 +2776,25 @@
         <v>0</v>
       </c>
       <c r="C55">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D55">
+        <v>6</v>
+      </c>
+      <c r="E55">
+        <v>0</v>
+      </c>
+      <c r="F55">
+        <v>0</v>
+      </c>
+      <c r="G55">
         <v>7</v>
       </c>
-      <c r="E55">
-        <v>0</v>
-      </c>
-      <c r="F55">
-        <v>0</v>
-      </c>
-      <c r="G55">
-        <v>4</v>
-      </c>
       <c r="H55">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J55" t="s">
         <v>53</v>
@@ -2787,7 +2802,7 @@
     </row>
     <row r="56" spans="1:10" hidden="1">
       <c r="A56">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B56">
         <v>0</v>
@@ -2796,19 +2811,19 @@
         <v>23</v>
       </c>
       <c r="D56">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E56">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F56">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G56">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H56">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="I56">
         <v>0</v>
@@ -2817,33 +2832,33 @@
         <v>54</v>
       </c>
     </row>
-    <row r="57" spans="1:10">
+    <row r="57" spans="1:10" hidden="1">
       <c r="A57">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B57">
         <v>1</v>
       </c>
       <c r="C57">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="D57">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="E57">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F57">
         <v>0</v>
       </c>
       <c r="G57">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="H57">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="I57">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J57" t="s">
         <v>55</v>
@@ -2851,28 +2866,28 @@
     </row>
     <row r="58" spans="1:10" hidden="1">
       <c r="A58">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B58">
         <v>1</v>
       </c>
       <c r="C58">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D58">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E58">
         <v>2</v>
       </c>
       <c r="F58">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G58">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H58">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I58">
         <v>0</v>
@@ -2889,10 +2904,10 @@
         <v>0</v>
       </c>
       <c r="C59">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D59">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="E59">
         <v>0</v>
@@ -2901,10 +2916,10 @@
         <v>0</v>
       </c>
       <c r="G59">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="H59">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="I59">
         <v>0</v>
@@ -2915,28 +2930,28 @@
     </row>
     <row r="60" spans="1:10" hidden="1">
       <c r="A60">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B60">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C60">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D60">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E60">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F60">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G60">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="H60">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="I60">
         <v>0</v>
@@ -2953,10 +2968,10 @@
         <v>0</v>
       </c>
       <c r="C61">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D61">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E61">
         <v>0</v>
@@ -2965,10 +2980,10 @@
         <v>0</v>
       </c>
       <c r="G61">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H61">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="I61">
         <v>0</v>
@@ -2979,7 +2994,7 @@
     </row>
     <row r="62" spans="1:10" hidden="1">
       <c r="A62">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B62">
         <v>1</v>
@@ -2988,19 +3003,19 @@
         <v>2</v>
       </c>
       <c r="D62">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E62">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F62">
         <v>1</v>
       </c>
       <c r="G62">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H62">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I62">
         <v>0</v>
@@ -3009,15 +3024,15 @@
         <v>60</v>
       </c>
     </row>
-    <row r="63" spans="1:10">
+    <row r="63" spans="1:10" hidden="1">
       <c r="A63">
         <v>3</v>
       </c>
       <c r="B63">
+        <v>3</v>
+      </c>
+      <c r="C63">
         <v>8</v>
-      </c>
-      <c r="C63">
-        <v>10</v>
       </c>
       <c r="D63">
         <v>2</v>
@@ -3026,22 +3041,22 @@
         <v>3</v>
       </c>
       <c r="F63">
+        <v>4</v>
+      </c>
+      <c r="G63">
+        <v>14</v>
+      </c>
+      <c r="H63">
         <v>9</v>
       </c>
-      <c r="G63">
-        <v>16</v>
-      </c>
-      <c r="H63">
-        <v>19</v>
-      </c>
       <c r="I63">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J63" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="64" spans="1:10" hidden="1">
+    <row r="64" spans="1:10">
       <c r="A64">
         <v>0</v>
       </c>
@@ -3049,10 +3064,10 @@
         <v>0</v>
       </c>
       <c r="C64">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="D64">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E64">
         <v>0</v>
@@ -3061,13 +3076,13 @@
         <v>0</v>
       </c>
       <c r="G64">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="H64">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I64">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J64" t="s">
         <v>62</v>
@@ -3078,37 +3093,31 @@
         <v>0</v>
       </c>
       <c r="B65">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C65">
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="D65">
         <v>47</v>
       </c>
       <c r="E65">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F65">
         <v>0</v>
       </c>
       <c r="G65">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="H65">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="I65">
         <v>0</v>
       </c>
       <c r="J65" t="s">
         <v>63</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10">
-      <c r="I66">
-        <f>SUM(I10:I63)</f>
-        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>